<commit_message>
Update Auto Scaling Policy
</commit_message>
<xml_diff>
--- a/load_test/RPS Tests.xlsx
+++ b/load_test/RPS Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UNCC\20Sp_DSBA 6190 (Intro to Cloud Computing)\Project\Team Project\load_test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6569653F-2E37-49C0-A1E5-1DE149711D4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A506C961-C542-4878-84C0-F780E0777FDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-975" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{375728E7-35F2-4163-A08A-3A2696897029}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{375728E7-35F2-4163-A08A-3A2696897029}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Slave Instance</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Plan</t>
+  </si>
+  <si>
+    <t>Time (min)</t>
+  </si>
+  <si>
+    <t>Time (sec)</t>
   </si>
 </sst>
 </file>
@@ -484,8 +490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71088B10-8726-47D1-B5CA-834E89F02CF3}">
   <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1140,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AA52F70-39C9-4704-BCA4-92F3982BD479}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R18" sqref="R18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,6 +1157,8 @@
     <col min="1" max="1" width="38.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1580,7 +1588,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
         <f>A16</f>
         <v>30000</v>
@@ -1612,7 +1620,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
         <f>A17</f>
         <v>30000</v>
@@ -1644,7 +1652,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
         <f>A18</f>
         <v>30000</v>
@@ -1676,7 +1684,7 @@
         <v>2.4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
         <f>A19</f>
         <v>30000</v>
@@ -1708,12 +1716,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1738,8 +1746,14 @@
       <c r="H25" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J25" t="s">
+        <v>25</v>
+      </c>
+      <c r="K25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>30000</v>
       </c>
@@ -1768,8 +1782,15 @@
         <f>G26/A26</f>
         <v>0.6</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <f>J26*60</f>
+        <v>300</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
         <f>A26</f>
         <v>30000</v>
@@ -1799,8 +1820,15 @@
         <f>G27/A27</f>
         <v>1.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>10</v>
+      </c>
+      <c r="K27">
+        <f>J27*60</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
         <f>A27</f>
         <v>30000</v>
@@ -1829,6 +1857,13 @@
       <c r="H28">
         <f>G28/A28</f>
         <v>2.4</v>
+      </c>
+      <c r="J28">
+        <v>10</v>
+      </c>
+      <c r="K28">
+        <f>J28*60</f>
+        <v>600</v>
       </c>
     </row>
   </sheetData>

</xml_diff>